<commit_message>
JK: add reestr info by childs
</commit_message>
<xml_diff>
--- a/modules/jk/files/orders.xlsx
+++ b/modules/jk/files/orders.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="102">
   <si>
     <t xml:space="preserve">№ п/п</t>
   </si>
@@ -101,6 +101,15 @@
     <t xml:space="preserve">Супруга</t>
   </si>
   <si>
+    <t xml:space="preserve">Ребёнок 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ребёнок 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ребёнок 3</t>
+  </si>
+  <si>
     <t xml:space="preserve">Наименование МРФ/РФ</t>
   </si>
   <si>
@@ -263,6 +272,18 @@
     <t xml:space="preserve">Трудоустройство</t>
   </si>
   <si>
+    <t xml:space="preserve">Свидетельство о рождении</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Паспорт</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ребёнок студент</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ребёнок инвалид</t>
+  </si>
+  <si>
     <t xml:space="preserve">Сумма, тыс. руб.</t>
   </si>
   <si>
@@ -303,6 +324,12 @@
   </si>
   <si>
     <t xml:space="preserve">Находится в декретном отпуске</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Подразделение выдачи</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Адрес регистрации ребёнка совпадает с адресом регистрации</t>
   </si>
 </sst>
 </file>
@@ -352,7 +379,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -387,6 +414,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF00CC"/>
         <bgColor rgb="FFFF00FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF66CC"/>
+        <bgColor rgb="FFFF99CC"/>
       </patternFill>
     </fill>
   </fills>
@@ -431,7 +464,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -452,6 +485,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -469,6 +506,10 @@
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -516,7 +557,7 @@
       <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FFFF66CC"/>
       <rgbColor rgb="FF0066CC"/>
       <rgbColor rgb="FFD9D9D9"/>
       <rgbColor rgb="FF000080"/>
@@ -565,10 +606,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:CD155"/>
+  <dimension ref="A1:DZ155"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="BP1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="BT8" activeCellId="0" sqref="BT8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -577,7 +622,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="37.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="59.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="59.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="10.85"/>
@@ -633,446 +678,743 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="78" min="74" style="2" width="9.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="79" min="79" style="2" width="16.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="82" min="80" style="2" width="17.98"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="83" style="5" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="83" min="83" style="2" width="36.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="84" min="84" style="2" width="17.3"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="88" min="85" style="2" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="89" min="89" style="2" width="28.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="90" min="90" style="2" width="33.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="91" min="91" style="2" width="42.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="92" min="92" style="5" width="15.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="94" min="93" style="5" width="16.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="95" min="95" style="5" width="30.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="96" min="96" style="5" width="19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="98" min="97" style="5" width="11.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="99" min="99" style="2" width="36.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="100" min="100" style="2" width="17.3"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="104" min="101" style="2" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="105" min="105" style="2" width="28.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="106" min="106" style="2" width="33.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="107" min="107" style="2" width="42.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="108" min="108" style="5" width="15.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="110" min="109" style="5" width="16.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="111" min="111" style="5" width="30.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="112" min="112" style="5" width="19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="114" min="113" style="5" width="11.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="115" min="115" style="2" width="36.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="116" min="116" style="2" width="17.3"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="120" min="117" style="2" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="121" min="121" style="2" width="28.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="122" min="122" style="2" width="33.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="123" min="123" style="2" width="42.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="124" min="124" style="5" width="15.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="126" min="125" style="5" width="16.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="127" min="127" style="5" width="30.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="128" min="128" style="5" width="19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="130" min="129" style="5" width="11.36"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="131" style="6" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" s="10" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
+    <row r="1" s="12" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="7" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7" t="s">
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7"/>
-      <c r="W1" s="7"/>
-      <c r="X1" s="7"/>
-      <c r="Y1" s="7"/>
-      <c r="Z1" s="7"/>
-      <c r="AA1" s="7"/>
-      <c r="AB1" s="7"/>
-      <c r="AC1" s="7" t="s">
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="8"/>
+      <c r="AA1" s="8"/>
+      <c r="AB1" s="8"/>
+      <c r="AC1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="AD1" s="7" t="s">
+      <c r="AD1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="AE1" s="7" t="s">
+      <c r="AE1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="AF1" s="6" t="s">
+      <c r="AF1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="AG1" s="7" t="s">
+      <c r="AG1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="AH1" s="7"/>
-      <c r="AI1" s="7"/>
-      <c r="AJ1" s="7"/>
-      <c r="AK1" s="7"/>
-      <c r="AL1" s="7"/>
-      <c r="AM1" s="7"/>
-      <c r="AN1" s="7"/>
-      <c r="AO1" s="7"/>
-      <c r="AP1" s="7"/>
-      <c r="AQ1" s="7"/>
-      <c r="AR1" s="7" t="s">
+      <c r="AH1" s="8"/>
+      <c r="AI1" s="8"/>
+      <c r="AJ1" s="8"/>
+      <c r="AK1" s="8"/>
+      <c r="AL1" s="8"/>
+      <c r="AM1" s="8"/>
+      <c r="AN1" s="8"/>
+      <c r="AO1" s="8"/>
+      <c r="AP1" s="8"/>
+      <c r="AQ1" s="8"/>
+      <c r="AR1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="AS1" s="7"/>
-      <c r="AT1" s="7"/>
-      <c r="AU1" s="7"/>
-      <c r="AV1" s="7"/>
-      <c r="AW1" s="7"/>
-      <c r="AX1" s="7" t="s">
+      <c r="AS1" s="8"/>
+      <c r="AT1" s="8"/>
+      <c r="AU1" s="8"/>
+      <c r="AV1" s="8"/>
+      <c r="AW1" s="8"/>
+      <c r="AX1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="AY1" s="7"/>
-      <c r="AZ1" s="7"/>
-      <c r="BA1" s="7"/>
-      <c r="BB1" s="7" t="s">
+      <c r="AY1" s="8"/>
+      <c r="AZ1" s="8"/>
+      <c r="BA1" s="8"/>
+      <c r="BB1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="BC1" s="7" t="s">
+      <c r="BC1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="BD1" s="7" t="s">
+      <c r="BD1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="BE1" s="7" t="s">
+      <c r="BE1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="BF1" s="7" t="s">
+      <c r="BF1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="BG1" s="7" t="s">
+      <c r="BG1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="BH1" s="7" t="s">
+      <c r="BH1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="BI1" s="7" t="s">
+      <c r="BI1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="BJ1" s="7" t="s">
+      <c r="BJ1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="BK1" s="7" t="s">
+      <c r="BK1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="BL1" s="7" t="s">
+      <c r="BL1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="BM1" s="8" t="s">
+      <c r="BM1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="BN1" s="8" t="s">
+      <c r="BN1" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="BO1" s="8"/>
-      <c r="BP1" s="8" t="s">
+      <c r="BO1" s="9"/>
+      <c r="BP1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="BQ1" s="9" t="s">
+      <c r="BQ1" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="BR1" s="9"/>
-      <c r="BS1" s="9"/>
-      <c r="BT1" s="9"/>
-      <c r="BU1" s="9"/>
-      <c r="BV1" s="9"/>
-      <c r="BW1" s="9"/>
-      <c r="BX1" s="9"/>
-      <c r="BY1" s="9"/>
-      <c r="BZ1" s="9"/>
-      <c r="CA1" s="9"/>
-      <c r="CB1" s="9"/>
-      <c r="CC1" s="9"/>
-      <c r="CD1" s="9"/>
+      <c r="BR1" s="10"/>
+      <c r="BS1" s="10"/>
+      <c r="BT1" s="10"/>
+      <c r="BU1" s="10"/>
+      <c r="BV1" s="10"/>
+      <c r="BW1" s="10"/>
+      <c r="BX1" s="10"/>
+      <c r="BY1" s="10"/>
+      <c r="BZ1" s="10"/>
+      <c r="CA1" s="10"/>
+      <c r="CB1" s="10"/>
+      <c r="CC1" s="10"/>
+      <c r="CD1" s="10"/>
+      <c r="CE1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="CF1" s="7"/>
+      <c r="CG1" s="7"/>
+      <c r="CH1" s="7"/>
+      <c r="CI1" s="7"/>
+      <c r="CJ1" s="7"/>
+      <c r="CK1" s="7"/>
+      <c r="CL1" s="7"/>
+      <c r="CM1" s="7"/>
+      <c r="CN1" s="7"/>
+      <c r="CO1" s="7"/>
+      <c r="CP1" s="7"/>
+      <c r="CQ1" s="7"/>
+      <c r="CR1" s="7"/>
+      <c r="CS1" s="7"/>
+      <c r="CT1" s="7"/>
+      <c r="CU1" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="CV1" s="11"/>
+      <c r="CW1" s="11"/>
+      <c r="CX1" s="11"/>
+      <c r="CY1" s="11"/>
+      <c r="CZ1" s="11"/>
+      <c r="DA1" s="11"/>
+      <c r="DB1" s="11"/>
+      <c r="DC1" s="11"/>
+      <c r="DD1" s="11"/>
+      <c r="DE1" s="11"/>
+      <c r="DF1" s="11"/>
+      <c r="DG1" s="11"/>
+      <c r="DH1" s="11"/>
+      <c r="DI1" s="11"/>
+      <c r="DJ1" s="11"/>
+      <c r="DK1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="DL1" s="7"/>
+      <c r="DM1" s="7"/>
+      <c r="DN1" s="7"/>
+      <c r="DO1" s="7"/>
+      <c r="DP1" s="7"/>
+      <c r="DQ1" s="7"/>
+      <c r="DR1" s="7"/>
+      <c r="DS1" s="7"/>
+      <c r="DT1" s="7"/>
+      <c r="DU1" s="7"/>
+      <c r="DV1" s="7"/>
+      <c r="DW1" s="7"/>
+      <c r="DX1" s="7"/>
+      <c r="DY1" s="7"/>
+      <c r="DZ1" s="7"/>
     </row>
-    <row r="2" s="10" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="7" t="s">
+    <row r="2" s="12" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="C2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="D2" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="E2" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="F2" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="G2" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="H2" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="I2" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="J2" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="K2" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="L2" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="P2" s="7" t="s">
+      <c r="M2" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="Q2" s="7" t="s">
+      <c r="N2" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="R2" s="7" t="s">
+      <c r="O2" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="S2" s="7" t="s">
+      <c r="P2" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="T2" s="7" t="s">
+      <c r="Q2" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="U2" s="7" t="s">
+      <c r="R2" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="V2" s="7" t="s">
+      <c r="S2" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="W2" s="7" t="s">
+      <c r="T2" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="X2" s="7" t="s">
+      <c r="U2" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="Y2" s="7" t="s">
+      <c r="V2" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="Z2" s="7" t="s">
+      <c r="W2" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="AA2" s="7" t="s">
+      <c r="X2" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="AB2" s="7" t="s">
+      <c r="Y2" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="AC2" s="7"/>
-      <c r="AD2" s="7"/>
-      <c r="AE2" s="7"/>
-      <c r="AF2" s="6"/>
-      <c r="AG2" s="7" t="s">
+      <c r="Z2" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="AH2" s="7" t="s">
+      <c r="AA2" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="AI2" s="7" t="s">
+      <c r="AB2" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="AJ2" s="7" t="s">
+      <c r="AC2" s="8"/>
+      <c r="AD2" s="8"/>
+      <c r="AE2" s="8"/>
+      <c r="AF2" s="7"/>
+      <c r="AG2" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="AK2" s="7" t="s">
+      <c r="AH2" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="AL2" s="7" t="s">
+      <c r="AI2" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="AM2" s="7" t="s">
+      <c r="AJ2" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="AN2" s="7" t="s">
+      <c r="AK2" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="AO2" s="7" t="s">
+      <c r="AL2" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="AP2" s="6" t="s">
+      <c r="AM2" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="AQ2" s="7" t="s">
+      <c r="AN2" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="AR2" s="7" t="s">
+      <c r="AO2" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="AS2" s="11" t="s">
+      <c r="AP2" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="AT2" s="11" t="s">
+      <c r="AQ2" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="AU2" s="7" t="s">
+      <c r="AR2" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="AV2" s="7" t="s">
+      <c r="AS2" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="AW2" s="7"/>
-      <c r="AX2" s="12" t="s">
+      <c r="AT2" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="AY2" s="7" t="s">
+      <c r="AU2" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="AZ2" s="7" t="s">
+      <c r="AV2" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="BA2" s="7" t="s">
+      <c r="AW2" s="8"/>
+      <c r="AX2" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="BB2" s="7"/>
-      <c r="BC2" s="7"/>
-      <c r="BD2" s="7"/>
-      <c r="BE2" s="7"/>
-      <c r="BF2" s="7"/>
-      <c r="BG2" s="7"/>
-      <c r="BH2" s="7"/>
-      <c r="BI2" s="7"/>
-      <c r="BJ2" s="7"/>
-      <c r="BK2" s="7"/>
-      <c r="BL2" s="7"/>
-      <c r="BM2" s="8"/>
-      <c r="BN2" s="8" t="s">
+      <c r="AY2" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="BO2" s="8" t="s">
+      <c r="AZ2" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="BP2" s="8"/>
-      <c r="BQ2" s="9" t="s">
+      <c r="BA2" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="BR2" s="9" t="s">
+      <c r="BB2" s="8"/>
+      <c r="BC2" s="8"/>
+      <c r="BD2" s="8"/>
+      <c r="BE2" s="8"/>
+      <c r="BF2" s="8"/>
+      <c r="BG2" s="8"/>
+      <c r="BH2" s="8"/>
+      <c r="BI2" s="8"/>
+      <c r="BJ2" s="8"/>
+      <c r="BK2" s="8"/>
+      <c r="BL2" s="8"/>
+      <c r="BM2" s="9"/>
+      <c r="BN2" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="BS2" s="9" t="s">
+      <c r="BO2" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="BT2" s="9"/>
-      <c r="BU2" s="9"/>
-      <c r="BV2" s="9" t="s">
+      <c r="BP2" s="9"/>
+      <c r="BQ2" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="BW2" s="9"/>
-      <c r="BX2" s="9"/>
-      <c r="BY2" s="9"/>
-      <c r="BZ2" s="9"/>
-      <c r="CA2" s="9"/>
-      <c r="CB2" s="9" t="s">
+      <c r="BR2" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="CC2" s="9"/>
-      <c r="CD2" s="9"/>
+      <c r="BS2" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="BT2" s="10"/>
+      <c r="BU2" s="10"/>
+      <c r="BV2" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="BW2" s="10"/>
+      <c r="BX2" s="10"/>
+      <c r="BY2" s="10"/>
+      <c r="BZ2" s="10"/>
+      <c r="CA2" s="10"/>
+      <c r="CB2" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="CC2" s="10"/>
+      <c r="CD2" s="10"/>
+      <c r="CE2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="CF2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="CG2" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="CH2" s="7"/>
+      <c r="CI2" s="7"/>
+      <c r="CJ2" s="7"/>
+      <c r="CK2" s="7"/>
+      <c r="CL2" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="CM2" s="7"/>
+      <c r="CN2" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="CO2" s="7"/>
+      <c r="CP2" s="7"/>
+      <c r="CQ2" s="7"/>
+      <c r="CR2" s="7"/>
+      <c r="CS2" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="CT2" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="CU2" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="CV2" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="CW2" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="CX2" s="11"/>
+      <c r="CY2" s="11"/>
+      <c r="CZ2" s="11"/>
+      <c r="DA2" s="11"/>
+      <c r="DB2" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="DC2" s="11"/>
+      <c r="DD2" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="DE2" s="11"/>
+      <c r="DF2" s="11"/>
+      <c r="DG2" s="11"/>
+      <c r="DH2" s="11"/>
+      <c r="DI2" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="DJ2" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="DK2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="DL2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="DM2" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="DN2" s="7"/>
+      <c r="DO2" s="7"/>
+      <c r="DP2" s="7"/>
+      <c r="DQ2" s="7"/>
+      <c r="DR2" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="DS2" s="7"/>
+      <c r="DT2" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="DU2" s="7"/>
+      <c r="DV2" s="7"/>
+      <c r="DW2" s="7"/>
+      <c r="DX2" s="7"/>
+      <c r="DY2" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="DZ2" s="7" t="s">
+        <v>85</v>
+      </c>
     </row>
-    <row r="3" s="10" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7"/>
-      <c r="T3" s="7"/>
-      <c r="U3" s="7"/>
-      <c r="V3" s="7"/>
-      <c r="W3" s="7"/>
-      <c r="X3" s="7"/>
-      <c r="Y3" s="7"/>
-      <c r="Z3" s="7"/>
-      <c r="AA3" s="7"/>
-      <c r="AB3" s="7"/>
-      <c r="AC3" s="7"/>
-      <c r="AD3" s="7"/>
-      <c r="AE3" s="7"/>
-      <c r="AF3" s="6"/>
-      <c r="AG3" s="7"/>
-      <c r="AH3" s="7"/>
-      <c r="AI3" s="7"/>
-      <c r="AJ3" s="7"/>
-      <c r="AK3" s="7"/>
-      <c r="AL3" s="7"/>
-      <c r="AM3" s="7"/>
-      <c r="AN3" s="7"/>
-      <c r="AO3" s="7"/>
-      <c r="AP3" s="6"/>
-      <c r="AQ3" s="7"/>
-      <c r="AR3" s="7"/>
-      <c r="AS3" s="11"/>
-      <c r="AT3" s="11"/>
-      <c r="AU3" s="7"/>
-      <c r="AV3" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="AW3" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="AX3" s="12"/>
-      <c r="AY3" s="7"/>
-      <c r="AZ3" s="7"/>
-      <c r="BA3" s="7"/>
-      <c r="BB3" s="7"/>
-      <c r="BC3" s="7"/>
-      <c r="BD3" s="7"/>
-      <c r="BE3" s="7"/>
-      <c r="BF3" s="7"/>
-      <c r="BG3" s="7"/>
-      <c r="BH3" s="7"/>
-      <c r="BI3" s="7"/>
-      <c r="BJ3" s="7"/>
-      <c r="BK3" s="7"/>
-      <c r="BL3" s="7"/>
-      <c r="BM3" s="8"/>
-      <c r="BN3" s="8"/>
-      <c r="BO3" s="8"/>
-      <c r="BP3" s="8"/>
-      <c r="BQ3" s="9"/>
-      <c r="BR3" s="9"/>
-      <c r="BS3" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="BT3" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="BU3" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="BV3" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="BW3" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="BX3" s="9" t="s">
+    <row r="3" s="12" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="8"/>
+      <c r="AC3" s="8"/>
+      <c r="AD3" s="8"/>
+      <c r="AE3" s="8"/>
+      <c r="AF3" s="7"/>
+      <c r="AG3" s="8"/>
+      <c r="AH3" s="8"/>
+      <c r="AI3" s="8"/>
+      <c r="AJ3" s="8"/>
+      <c r="AK3" s="8"/>
+      <c r="AL3" s="8"/>
+      <c r="AM3" s="8"/>
+      <c r="AN3" s="8"/>
+      <c r="AO3" s="8"/>
+      <c r="AP3" s="7"/>
+      <c r="AQ3" s="8"/>
+      <c r="AR3" s="8"/>
+      <c r="AS3" s="13"/>
+      <c r="AT3" s="13"/>
+      <c r="AU3" s="8"/>
+      <c r="AV3" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="BY3" s="9" t="s">
+      <c r="AW3" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="BZ3" s="9" t="s">
+      <c r="AX3" s="14"/>
+      <c r="AY3" s="8"/>
+      <c r="AZ3" s="8"/>
+      <c r="BA3" s="8"/>
+      <c r="BB3" s="8"/>
+      <c r="BC3" s="8"/>
+      <c r="BD3" s="8"/>
+      <c r="BE3" s="8"/>
+      <c r="BF3" s="8"/>
+      <c r="BG3" s="8"/>
+      <c r="BH3" s="8"/>
+      <c r="BI3" s="8"/>
+      <c r="BJ3" s="8"/>
+      <c r="BK3" s="8"/>
+      <c r="BL3" s="8"/>
+      <c r="BM3" s="9"/>
+      <c r="BN3" s="9"/>
+      <c r="BO3" s="9"/>
+      <c r="BP3" s="9"/>
+      <c r="BQ3" s="10"/>
+      <c r="BR3" s="10"/>
+      <c r="BS3" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="CA3" s="9" t="s">
+      <c r="BT3" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="CB3" s="9" t="s">
+      <c r="BU3" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="CC3" s="9" t="s">
+      <c r="BV3" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="CD3" s="9" t="s">
+      <c r="BW3" s="10" t="s">
         <v>92</v>
       </c>
+      <c r="BX3" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="BY3" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="BZ3" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="CA3" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="CB3" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="CC3" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="CD3" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="CE3" s="7"/>
+      <c r="CF3" s="7"/>
+      <c r="CG3" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="CH3" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="CI3" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="CJ3" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="CK3" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="CL3" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="CM3" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="CN3" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="CO3" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="CP3" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="CQ3" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="CR3" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="CS3" s="7"/>
+      <c r="CT3" s="7"/>
+      <c r="CU3" s="11"/>
+      <c r="CV3" s="11"/>
+      <c r="CW3" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="CX3" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="CY3" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="CZ3" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="DA3" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="DB3" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="DC3" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="DD3" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="DE3" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="DF3" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="DG3" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="DH3" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="DI3" s="11"/>
+      <c r="DJ3" s="11"/>
+      <c r="DK3" s="7"/>
+      <c r="DL3" s="7"/>
+      <c r="DM3" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="DN3" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="DO3" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="DP3" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="DQ3" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="DR3" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="DS3" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="DT3" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="DU3" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="DV3" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="DW3" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="DX3" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="DY3" s="7"/>
+      <c r="DZ3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="54.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="5" customFormat="false" ht="54.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1228,7 +1570,7 @@
     <row r="155" customFormat="false" ht="54.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <autoFilter ref="B1:B3"/>
-  <mergeCells count="77">
+  <mergeCells count="97">
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="D1:R1"/>
     <mergeCell ref="T1:AB1"/>
@@ -1254,6 +1596,9 @@
     <mergeCell ref="BN1:BO1"/>
     <mergeCell ref="BP1:BP3"/>
     <mergeCell ref="BQ1:CD1"/>
+    <mergeCell ref="CE1:CT1"/>
+    <mergeCell ref="CU1:DJ1"/>
+    <mergeCell ref="DK1:DZ1"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="D2:D3"/>
@@ -1303,9 +1648,26 @@
     <mergeCell ref="BA2:BA3"/>
     <mergeCell ref="BN2:BN3"/>
     <mergeCell ref="BO2:BO3"/>
+    <mergeCell ref="BQ2:BQ3"/>
+    <mergeCell ref="BR2:BR3"/>
     <mergeCell ref="BS2:BU2"/>
     <mergeCell ref="BV2:CA2"/>
     <mergeCell ref="CB2:CD2"/>
+    <mergeCell ref="CG2:CK2"/>
+    <mergeCell ref="CL2:CM2"/>
+    <mergeCell ref="CN2:CR2"/>
+    <mergeCell ref="CS2:CS3"/>
+    <mergeCell ref="CT2:CT3"/>
+    <mergeCell ref="CW2:DA2"/>
+    <mergeCell ref="DB2:DC2"/>
+    <mergeCell ref="DD2:DH2"/>
+    <mergeCell ref="DI2:DI3"/>
+    <mergeCell ref="DJ2:DJ3"/>
+    <mergeCell ref="DM2:DQ2"/>
+    <mergeCell ref="DR2:DS2"/>
+    <mergeCell ref="DT2:DX2"/>
+    <mergeCell ref="DY2:DY3"/>
+    <mergeCell ref="DZ2:DZ3"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.236111111111111" right="0.236111111111111" top="0.747916666666667" bottom="0.747916666666667" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>